<commit_message>
test(backend): update/add tests for better coverage
</commit_message>
<xml_diff>
--- a/backend/__tests_resources__/excel/BarChart_FullDetails.xlsx
+++ b/backend/__tests_resources__/excel/BarChart_FullDetails.xlsx
@@ -1,33 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nituv\OneDrive\Documents\GitHub\IllustryBackend\__tests_resources__\excel\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D0637F6-6BC9-462A-917F-8DCCBEAD455E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="32385" yWindow="1785" windowWidth="22290" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
+    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
+    <t>BarChart_FullDetails_SKIPPED</t>
+  </si>
+  <si>
+    <t>BarChart_FullDetails description</t>
+  </si>
+  <si>
     <t>full</t>
   </si>
   <si>
     <t>first</t>
   </si>
   <si>
+    <t>BarChart_FullDetails</t>
+  </si>
+  <si>
     <t>second</t>
   </si>
   <si>
@@ -35,44 +35,37 @@
   </si>
   <si>
     <t>forth</t>
-  </si>
-  <si>
-    <t>BarChart_FullDetails_SKIPPED</t>
-  </si>
-  <si>
-    <t>BarChart_FullDetails</t>
-  </si>
-  <si>
-    <t>BarChart_FullDetails description</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <fonts count="5">
     <font>
-      <sz val="10"/>
+      <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
+      <sz val="12.0"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="12.0"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <sz val="11.0"/>
+      <color rgb="FFCE9178"/>
+      <name val="Consolas"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFCE9178"/>
-      <name val="Consolas"/>
-      <family val="3"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
@@ -80,50 +73,51 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="lightGray"/>
     </fill>
   </fills>
   <borders count="1">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+  <cellXfs count="7">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -313,114 +307,120 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1521751-1AFA-49BD-8965-68FF5ADC042D}">
-  <dimension ref="A1:H4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col min="3" max="3" width="46.7109375" customWidth="1"/>
-    <col min="4" max="4" width="46" customWidth="1"/>
-    <col min="5" max="5" width="44" customWidth="1"/>
+    <col customWidth="1" min="2" max="2" width="32.63"/>
+    <col customWidth="1" min="4" max="4" width="29.0"/>
+    <col customWidth="1" min="5" max="5" width="26.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3">
+    <row r="1">
+      <c r="A1" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="B1" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="C1" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1">
+      <c r="F1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="4"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="C2" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1">
+      <c r="F2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="G2" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="H2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="I2" s="4"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="B3" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="C3" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" s="4"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="2">
+        <v>4.0</v>
+      </c>
+      <c r="B4" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="C4" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="H4" s="5" t="s">
         <v>7</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="G1">
-        <v>3</v>
-      </c>
-      <c r="H1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1">
-        <v>2</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>3</v>
-      </c>
-      <c r="H2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
-        <v>3</v>
-      </c>
-      <c r="B3" s="2">
-        <v>1</v>
-      </c>
-      <c r="C3" s="1">
-        <v>2</v>
-      </c>
-      <c r="G3">
-        <v>3</v>
-      </c>
-      <c r="H3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>4</v>
-      </c>
-      <c r="B4" s="2">
-        <v>1</v>
-      </c>
-      <c r="C4" s="1">
-        <v>2</v>
-      </c>
-      <c r="G4">
-        <v>3</v>
-      </c>
-      <c r="H4" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>